<commit_message>
info: 1. 使用 MyBatis 進行 CRUD 操作 2. 使用客製化 LocalDateTimeHandler 調整時間格式 3. 使用 XML 編寫 MyBatis 的 SQL 語句
</commit_message>
<xml_diff>
--- a/output/assets.xlsx
+++ b/output/assets.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -38,22 +38,13 @@
     <t>User</t>
   </si>
   <si>
-    <t>A010</t>
+    <t>A012</t>
   </si>
   <si>
-    <t>Office Chair</t>
+    <t>Laptop</t>
   </si>
   <si>
-    <t>2024-03-14</t>
-  </si>
-  <si>
-    <t>A034</t>
-  </si>
-  <si>
-    <t>Beads</t>
-  </si>
-  <si>
-    <t>2024-02-27</t>
+    <t>2024-03-13</t>
   </si>
   <si>
     <t>Total</t>
@@ -101,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -135,7 +126,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>8</v>
@@ -144,53 +135,27 @@
         <v>9</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>10</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>250.0</v>
+        <v>1200.0</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="0">
-        <v>28.0</v>
-      </c>
-      <c r="B3" t="s" s="0">
+      <c r="A3" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>13</v>
-      </c>
       <c r="F3" t="n" s="0">
-        <v>290.0</v>
-      </c>
-      <c r="G3" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="H3" t="n" s="0">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>540.0</v>
+        <v>1200.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>